<commit_message>
added several plots, and rbf error sheets
</commit_message>
<xml_diff>
--- a/plots/polynomial_training_error.xlsx
+++ b/plots/polynomial_training_error.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Backup" sheetId="2" r:id="rId1"/>
     <sheet name="Trainings Error" sheetId="1" r:id="rId2"/>
     <sheet name="Validation Error" sheetId="3" r:id="rId3"/>
+    <sheet name="rbf backup" sheetId="4" r:id="rId4"/>
+    <sheet name="rbf trainings errror" sheetId="5" r:id="rId5"/>
+    <sheet name="rbf validation errror" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027" refMode="R1C1"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="205">
   <si>
     <t xml:space="preserve">1.3959312636409864 </t>
   </si>
@@ -272,13 +275,382 @@
   </si>
   <si>
     <t>Degree</t>
+  </si>
+  <si>
+    <t>N Centers</t>
+  </si>
+  <si>
+    <t>Validation Error</t>
+  </si>
+  <si>
+    <t>Testing Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.174469463632379     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6342134154427308    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6220512364453881    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6205095084575466    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6076433121299515    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.37094992303622604   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.4102585244135535    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1954736658098675    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.20824263194507003   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.18098863940586898   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1646097137040078    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.15983111095953076   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1573834173281604    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1377978827324884    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.13654094231829628   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.13768491662682017   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.13495961872468804   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1337747622066005    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.13289990828400586   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.13149643422631266   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.12780680263607758   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.11422965309681622   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1117166065390467    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.10568708500313223   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.10962654527512246   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.09787347746260772   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.10567708514282699   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.09349861689357748   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.09843970929322907   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.08867348461878438   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.08022559265476036   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.06994299835112788   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.06957878884628514   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.06495903650417706   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.06216687589502927   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.061249583226244804 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0585315509539835    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.060509675330424416 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.054452916301053075 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.420375462918048  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2716780942747143  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0803145558748106     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8183521930443755     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7726427958876833     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7741441314697823     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8203645256558302     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5296397319383842     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.630249022820128  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2879598418720983     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3351743905750926     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.37406739527708777    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.398193964432448  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3908438663296047     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.357267678823065  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.38157089841624153    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3657448034594945     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3574779924118439     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.36979694159478965    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.37068297727637023    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.44967905610961467    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.39941523627377395    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.46749364484939787    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.8061337942383398     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8207355101980404     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.868446916823557  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.1270067397629164     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.6961827447690245     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.735330114807603  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.247672199347799  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.450124915964787  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0345253984289335     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.3886417242541724     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">255.36546758484252     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.324751436806533     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">128.41309509870158     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">632.7902002801715  </t>
+  </si>
+  <si>
+    <t>94.4302950020843</t>
+  </si>
+  <si>
+    <t>151.95088373388978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">427.3920594408368 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">304.6665721254332 </t>
+  </si>
+  <si>
+    <t>1.3239375372291953</t>
+  </si>
+  <si>
+    <t>1.2246905380357107</t>
+  </si>
+  <si>
+    <t>0.8558382289316525</t>
+  </si>
+  <si>
+    <t>0.7861645020985443</t>
+  </si>
+  <si>
+    <t>0.7823533115008087</t>
+  </si>
+  <si>
+    <t>0.8028477246380266</t>
+  </si>
+  <si>
+    <t>0.471278645340536</t>
+  </si>
+  <si>
+    <t>0.5617939453400826</t>
+  </si>
+  <si>
+    <t>0.33701300824089064</t>
+  </si>
+  <si>
+    <t>0.31840784744794115</t>
+  </si>
+  <si>
+    <t>0.35461469515891353</t>
+  </si>
+  <si>
+    <t>0.40525740050753706</t>
+  </si>
+  <si>
+    <t>0.3852073165781011</t>
+  </si>
+  <si>
+    <t>0.37686534850956094</t>
+  </si>
+  <si>
+    <t>0.36956517511443787</t>
+  </si>
+  <si>
+    <t>0.3676724405588042</t>
+  </si>
+  <si>
+    <t>0.3593903647461817</t>
+  </si>
+  <si>
+    <t>0.37384975231019024</t>
+  </si>
+  <si>
+    <t>0.3750622371482431</t>
+  </si>
+  <si>
+    <t>0.4293626572914165</t>
+  </si>
+  <si>
+    <t>0.4001799264896775</t>
+  </si>
+  <si>
+    <t>0.48139864681977196</t>
+  </si>
+  <si>
+    <t>2.4897418062471894</t>
+  </si>
+  <si>
+    <t>1.1273533941875211</t>
+  </si>
+  <si>
+    <t>6.5883849545748365</t>
+  </si>
+  <si>
+    <t>5.256500958435373</t>
+  </si>
+  <si>
+    <t>9.108458859026836</t>
+  </si>
+  <si>
+    <t>5.56950144375552</t>
+  </si>
+  <si>
+    <t>6.554092692156446</t>
+  </si>
+  <si>
+    <t>3.679272038257757</t>
+  </si>
+  <si>
+    <t>1.6245562336699206</t>
+  </si>
+  <si>
+    <t>2.869101902481147</t>
+  </si>
+  <si>
+    <t>302.4139014886923</t>
+  </si>
+  <si>
+    <t>27.83748277743362</t>
+  </si>
+  <si>
+    <t>138.6954163634201</t>
+  </si>
+  <si>
+    <t>112.66606986300447</t>
+  </si>
+  <si>
+    <t>130.00545419127988</t>
+  </si>
+  <si>
+    <t>369.33897354816963</t>
+  </si>
+  <si>
+    <t>295.1071341927336</t>
+  </si>
+  <si>
+    <t>181.6718279531847</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,8 +666,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +712,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -329,6 +743,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -360,7 +780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,16 +792,59 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1155,7 +1618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -2076,4 +2539,1794 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:D41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="26">
+        <v>9</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>10</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>12</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>15</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24">
+        <v>16</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>18</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34">
+        <v>19</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>20</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>21</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20">
+        <v>22</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>23</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
+        <v>24</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>25</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>26</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>27</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22">
+        <v>28</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
+        <v>29</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>30</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <v>31</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <v>32</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="28">
+        <v>33</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>34</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="32">
+        <v>35</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>36</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
+        <v>37</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <v>38</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>39</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="30">
+        <v>40</v>
+      </c>
+      <c r="B41" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="A1:D41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="30">
+        <v>40</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>38</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>39</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>37</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>36</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="32">
+        <v>35</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>34</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="28">
+        <v>33</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>32</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>31</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>29</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>27</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>30</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="22">
+        <v>28</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>25</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>26</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>24</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>23</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="20">
+        <v>22</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>21</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>20</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="34">
+        <v>19</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>18</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="24">
+        <v>16</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>17</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>15</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>14</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
+        <v>13</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
+        <v>12</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>11</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="26">
+        <v>9</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <v>10</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
+        <v>7</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>8</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>6</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>5</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
+        <v>4</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <v>3</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>2</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="18">
+        <v>1</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D41">
+    <sortCondition ref="B2:B41"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
+        <v>9</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>10</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>14</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>17</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>16</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>18</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="34">
+        <v>19</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>11</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>15</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>13</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>12</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>21</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>20</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
+        <v>22</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>7</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>8</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>4</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>5</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>3</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>6</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>24</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>31</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>2</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
+        <v>1</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>23</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="32">
+        <v>35</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>37</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
+        <v>32</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
+        <v>30</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>34</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="28">
+        <v>33</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <v>26</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="22">
+        <v>28</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="30">
+        <v>40</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>25</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>39</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
+        <v>29</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <v>27</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>38</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="15">
+        <v>36</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D41">
+    <sortCondition ref="C2:C41"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added good pair plots
</commit_message>
<xml_diff>
--- a/plots/polynomial_training_error.xlsx
+++ b/plots/polynomial_training_error.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Backup" sheetId="2" r:id="rId1"/>
@@ -793,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -859,6 +859,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3752,7 +3753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -4347,10 +4348,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4399,6 +4400,13 @@
         <v>12.5</v>
       </c>
     </row>
+    <row r="8" spans="1:2" s="37" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="36"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="36"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>